<commit_message>
added targets to ci
</commit_message>
<xml_diff>
--- a/geometry_source/targets/rgd_runs.xlsx
+++ b/geometry_source/targets/rgd_runs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/opt/projects/gemc/clas12Tags/geometry_source/targets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC63113B-AE95-C246-A997-2F3BE555C7FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7919E290-0A4D-CA42-BE15-E437E53503E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="55580" yWindow="4940" windowWidth="41120" windowHeight="24420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18600" yWindow="780" windowWidth="31020" windowHeight="24800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
@@ -344,7 +344,7 @@
   <dimension ref="A1:D1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6548,7 +6548,7 @@
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D1000">
-    <sortCondition ref="D2:D1000"/>
+    <sortCondition ref="B2:B1000"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>